<commit_message>
bug fixes with data scraping
wrong columns being pulled in again.
</commit_message>
<xml_diff>
--- a/Scraping Scripts and Template/Time Related Features.xlsx
+++ b/Scraping Scripts and Template/Time Related Features.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="73">
   <si>
     <t>Year</t>
   </si>
@@ -210,6 +210,39 @@
   </si>
   <si>
     <t>2018-05-27</t>
+  </si>
+  <si>
+    <t>2006-04-21</t>
+  </si>
+  <si>
+    <t>2006-05-04</t>
+  </si>
+  <si>
+    <t>2006-05-18</t>
+  </si>
+  <si>
+    <t>2006-06-04</t>
+  </si>
+  <si>
+    <t>2007-04-11</t>
+  </si>
+  <si>
+    <t>2007-04-24</t>
+  </si>
+  <si>
+    <t>2007-05-09</t>
+  </si>
+  <si>
+    <t>2006-05-27</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>2019-04-10</t>
+  </si>
+  <si>
+    <t>2019-04-24</t>
   </si>
 </sst>
 </file>
@@ -535,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="A1:D34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,508 +597,564 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="2">
+        <v>2006</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="2">
+        <v>2006</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="2">
+        <v>2006</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="2">
+        <v>2007</v>
+      </c>
+      <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="2">
+        <v>2007</v>
+      </c>
+      <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="2">
+        <v>2007</v>
+      </c>
+      <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>2017</v>
+      <c r="A30" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>2017</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D38" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-    </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
+      <c r="A41" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
@@ -1091,6 +1180,42 @@
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>